<commit_message>
intrusion_test excel file making easier to read the topic words
</commit_message>
<xml_diff>
--- a/Intrusion_test.xlsx
+++ b/Intrusion_test.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miric\Documents\GitHub\smda_final_project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970385AB-5784-489B-8574-39F9CD7D3340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="720" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -28,16 +37,6 @@
 video</t>
   </si>
   <si>
-    <t xml:space="preserve">Topic 1:
-work
-interview
-job
-grammar
-hour
-document
-</t>
-  </si>
-  <si>
     <t>Topic 2:
 google
 description
@@ -112,23 +111,33 @@
   <si>
     <t>hour</t>
   </si>
+  <si>
+    <t>Topic 1:
+work
+interview
+job
+grammar
+hour
+document</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0&quot; / 6&quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -139,46 +148,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -368,183 +379,186 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="16" width="18.88"/>
+    <col min="1" max="16" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45528.813888888886</v>
+      </c>
+      <c r="B2" s="3">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>45528.813888888886</v>
-      </c>
-      <c r="B2" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="C2" s="5" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45528.814687500002</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45528.824062500003</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45528.825243055559</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>45528.8146875</v>
-      </c>
-      <c r="B3" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>45528.8240625</v>
-      </c>
-      <c r="B4" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="5">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3">
-        <v>45528.82524305556</v>
-      </c>
-      <c r="B5" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="5">
-        <v>1.0</v>
+      <c r="J5" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>